<commit_message>
updated product list, added images
</commit_message>
<xml_diff>
--- a/Docs/ProduktePreisliste.xlsx
+++ b/Docs/ProduktePreisliste.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>Weichbrötchen Webshop</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Barbecue</t>
   </si>
   <si>
-    <t>Majonnaise</t>
-  </si>
-  <si>
     <t>Ketchup</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>Vegiburger</t>
   </si>
   <si>
-    <t>Weichbrötchen, Rindfleischburger, Chedar, Gurke</t>
-  </si>
-  <si>
     <t>Gurke</t>
   </si>
   <si>
@@ -111,10 +105,25 @@
     <t>Country Fries</t>
   </si>
   <si>
-    <t>Potatoes</t>
-  </si>
-  <si>
     <t>Gemischter Salat</t>
+  </si>
+  <si>
+    <t>Mayonnaise</t>
+  </si>
+  <si>
+    <t>Cocktail</t>
+  </si>
+  <si>
+    <t>Curry</t>
+  </si>
+  <si>
+    <t>Weichbrötchen, Rindfleischburger, Cheddar, Gurke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension </t>
+  </si>
+  <si>
+    <t>Tomate</t>
   </si>
 </sst>
 </file>
@@ -453,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,7 +513,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -522,10 +531,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -535,45 +544,45 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
         <v>28</v>
-      </c>
-      <c r="B12" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -581,7 +590,7 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -589,7 +598,7 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -597,7 +606,7 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -605,15 +614,23 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -621,7 +638,7 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -629,7 +646,7 @@
         <v>14</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -637,7 +654,7 @@
         <v>14</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -645,7 +662,7 @@
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -653,7 +670,15 @@
         <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>